<commit_message>
Adding Default Feed Cost Data
</commit_message>
<xml_diff>
--- a/Feed Inputs/default_feeds.xlsx
+++ b/Feed Inputs/default_feeds.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradenlimb/CloudStation/Sustainability Science:Consulting/2024-10 RuFaS/SS-RuFaS Github/Feed Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDC5860-0D57-4345-8DAD-424EE8C06051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F759B6-7044-824B-88B2-67278FC7AF94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36140" yWindow="2560" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="calf_feeds" sheetId="1" r:id="rId1"/>
@@ -34,6 +34,77 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={EAE00DF7-B86E-3644-BB4F-D21A35FF781C}</author>
+    <author>tc={398F2569-DB3F-7740-AED6-DF3C9C869ACA}</author>
+    <author>Microsoft Office User</author>
+    <author>tc={13FEE7F8-26B9-B246-B915-13834D174CE6}</author>
+  </authors>
+  <commentList>
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{EAE00DF7-B86E-3644-BB4F-D21A35FF781C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Barley silage estimate from scaling factor from beefreserach.ca</t>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="1" shapeId="0" xr:uid="{398F2569-DB3F-7740-AED6-DF3C9C869ACA}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Scaled from corn silage for alfalfa silage</t>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="2" shapeId="0" xr:uid="{742043B9-D479-B948-BF16-E9420383C9D3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">scaled from 2009 report values
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B10" authorId="3" shapeId="0" xr:uid="{13FEE7F8-26B9-B246-B915-13834D174CE6}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Retail milk prices</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -376,7 +447,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -392,8 +463,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -415,6 +499,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -446,7 +536,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -454,6 +544,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,6 +560,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Braden Limb" id="{23496C3F-2903-264A-98C6-DDFB11FDD9F5}" userId="e37597ec4f9891ff" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -756,6 +853,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B6" dT="2025-03-13T20:50:15.08" personId="{23496C3F-2903-264A-98C6-DDFB11FDD9F5}" id="{EAE00DF7-B86E-3644-BB4F-D21A35FF781C}">
+    <text>Barley silage estimate from scaling factor from beefreserach.ca</text>
+  </threadedComment>
+  <threadedComment ref="B7" dT="2025-03-13T19:08:44.50" personId="{23496C3F-2903-264A-98C6-DDFB11FDD9F5}" id="{398F2569-DB3F-7740-AED6-DF3C9C869ACA}">
+    <text>Scaled from corn silage for alfalfa silage</text>
+  </threadedComment>
+  <threadedComment ref="B10" dT="2025-03-13T19:55:20.17" personId="{23496C3F-2903-264A-98C6-DDFB11FDD9F5}" id="{13FEE7F8-26B9-B246-B915-13834D174CE6}">
+    <text>Retail milk prices</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CL3"/>
@@ -8966,11 +9077,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:CL13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9280,7 +9391,7 @@
       <c r="A2">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C2" t="s">
@@ -10096,7 +10207,7 @@
       <c r="A5">
         <v>94</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>110</v>
       </c>
       <c r="C5" t="s">
@@ -10368,7 +10479,7 @@
       <c r="A6">
         <v>100</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>109</v>
       </c>
       <c r="C6" t="s">
@@ -10640,7 +10751,7 @@
       <c r="A7">
         <v>110</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>99</v>
       </c>
       <c r="C7" t="s">
@@ -11184,7 +11295,7 @@
       <c r="A9">
         <v>176</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>101</v>
       </c>
       <c r="C9" t="s">
@@ -12539,5 +12650,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Milk per CWT price recieved
</commit_message>
<xml_diff>
--- a/Feed Inputs/default_feeds.xlsx
+++ b/Feed Inputs/default_feeds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradenlimb/CloudStation/Sustainability Science:Consulting/2024-10 RuFaS/SS-RuFaS Github/Feed Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F759B6-7044-824B-88B2-67278FC7AF94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A321D6-B274-1F4C-BEFC-CEC30DE6D87B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9081,7 +9081,7 @@
   <dimension ref="A1:CL13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11295,7 +11295,7 @@
       <c r="A9">
         <v>176</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>101</v>
       </c>
       <c r="C9" t="s">

</xml_diff>